<commit_message>
Uppercase name for 5HT1E
</commit_message>
<xml_diff>
--- a/structure_data/construct_data/Stabilising_Mutations_In_Xtal_Constructs.xlsx
+++ b/structure_data/construct_data/Stabilising_Mutations_In_Xtal_Constructs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rwf545/Dropbox (GloriamGroup)/Projects_GPCRdb/GPCRdb_Proj_Construct_db/Annotation/Annotated_Mutations-David/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlt998/protwis_vagrant/shared/data/protwis/gpcr/structure_data/construct_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F047A56A-A616-E345-BE64-02A900F02337}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{43E2B6D4-95FE-6449-8C31-A01027F1C9E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9720" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28340" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mutation_Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mutation_Data!$G$1:$L$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Palmitoylation_removal!$B$1:$G$8</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6979" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7270" uniqueCount="553">
   <si>
     <t>AA no.</t>
   </si>
@@ -1740,6 +1740,87 @@
   </si>
   <si>
     <t>Phosphorylation site</t>
+  </si>
+  <si>
+    <t>6FKD</t>
+  </si>
+  <si>
+    <t>5KW2</t>
+  </si>
+  <si>
+    <t>6FK9</t>
+  </si>
+  <si>
+    <t>6FKC</t>
+  </si>
+  <si>
+    <t>6D35</t>
+  </si>
+  <si>
+    <t>q98sw5_xenla</t>
+  </si>
+  <si>
+    <t>2x54</t>
+  </si>
+  <si>
+    <t>6x77</t>
+  </si>
+  <si>
+    <t>5ZBQ</t>
+  </si>
+  <si>
+    <t>npy1r_human</t>
+  </si>
+  <si>
+    <t>6D32</t>
+  </si>
+  <si>
+    <t>5ZBH</t>
+  </si>
+  <si>
+    <t>5ZKP</t>
+  </si>
+  <si>
+    <t>ptafr_human</t>
+  </si>
+  <si>
+    <t>6x34</t>
+  </si>
+  <si>
+    <t>5V56</t>
+  </si>
+  <si>
+    <t>5ZKQ</t>
+  </si>
+  <si>
+    <t>6FK7</t>
+  </si>
+  <si>
+    <t>6FK6</t>
+  </si>
+  <si>
+    <t>6C1R</t>
+  </si>
+  <si>
+    <t>6C1Q</t>
+  </si>
+  <si>
+    <t>6FK8</t>
+  </si>
+  <si>
+    <t>6FKB</t>
+  </si>
+  <si>
+    <t>6FKA</t>
+  </si>
+  <si>
+    <t>5WB2</t>
+  </si>
+  <si>
+    <t>q80km9_hcmv</t>
+  </si>
+  <si>
+    <t>6GDG</t>
   </si>
 </sst>
 </file>
@@ -7354,8 +7435,8 @@
   <dimension ref="A1:X673"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A429" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B462" sqref="B462"/>
+      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC497" sqref="AC497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25801,7 +25882,7 @@
         <v>223</v>
       </c>
       <c r="V457" s="71" t="b">
-        <f t="shared" ref="V457:V496" si="8">AND(ISBLANK(M457),ISBLANK(N457),ISBLANK(O457),ISBLANK(P457),ISBLANK(Q457))</f>
+        <f t="shared" ref="V457:V520" si="8">AND(ISBLANK(M457),ISBLANK(N457),ISBLANK(O457),ISBLANK(P457),ISBLANK(Q457))</f>
         <v>0</v>
       </c>
       <c r="W457" s="71" t="s">
@@ -27540,46 +27621,1285 @@
       <c r="W496" s="36"/>
       <c r="X496" s="36"/>
     </row>
-    <row r="507" spans="7:9">
-      <c r="G507" s="41"/>
-      <c r="H507" s="42"/>
+    <row r="497" spans="2:22">
+      <c r="B497" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="G497" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H497" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J497" s="40">
+        <v>2</v>
+      </c>
+      <c r="K497" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L497" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R497" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V497" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" spans="2:22">
+      <c r="B498" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="G498" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H498" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J498" s="40">
+        <v>282</v>
+      </c>
+      <c r="K498" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L498" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R498" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V498" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="2:22">
+      <c r="B499" s="35" t="s">
+        <v>527</v>
+      </c>
+      <c r="G499" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="H499" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I499" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="J499" s="40">
+        <v>88</v>
+      </c>
+      <c r="K499" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L499" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R499" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V499" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="2:22">
+      <c r="B500" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G500" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H500" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J500" s="40">
+        <v>2</v>
+      </c>
+      <c r="K500" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L500" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R500" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V500" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="2:22">
+      <c r="B501" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G501" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H501" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J501" s="40">
+        <v>282</v>
+      </c>
+      <c r="K501" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L501" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R501" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V501" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="2:22">
+      <c r="B502" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="G502" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H502" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J502" s="40">
+        <v>2</v>
+      </c>
+      <c r="K502" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L502" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R502" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V502" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="2:22">
+      <c r="B503" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="G503" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H503" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J503" s="40">
+        <v>282</v>
+      </c>
+      <c r="K503" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L503" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R503" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V503" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" spans="2:22">
+      <c r="B504" s="35" t="s">
+        <v>530</v>
+      </c>
+      <c r="G504" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="H504" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J504" s="40">
+        <v>163</v>
+      </c>
+      <c r="K504" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L504" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R504" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V504" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" spans="2:22">
+      <c r="B505" s="35" t="s">
+        <v>530</v>
+      </c>
+      <c r="G505" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="H505" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I505" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="J505" s="40">
+        <v>227</v>
+      </c>
+      <c r="K505" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L505" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="R505" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V505" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" spans="2:22">
+      <c r="B506" s="35" t="s">
+        <v>530</v>
+      </c>
+      <c r="G506" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="H506" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I506" s="34" t="s">
+        <v>532</v>
+      </c>
+      <c r="J506" s="40">
+        <v>249</v>
+      </c>
+      <c r="K506" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L506" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R506" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V506" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="2:22">
+      <c r="B507" s="35" t="s">
+        <v>530</v>
+      </c>
+      <c r="G507" s="41" t="s">
+        <v>531</v>
+      </c>
+      <c r="H507" s="42" t="s">
+        <v>124</v>
+      </c>
       <c r="I507" s="43"/>
-    </row>
-    <row r="508" spans="7:9">
-      <c r="G508" s="41"/>
-      <c r="H508" s="42"/>
-      <c r="I508" s="43"/>
-    </row>
-    <row r="509" spans="7:9">
-      <c r="G509" s="41"/>
-      <c r="H509" s="42"/>
-      <c r="I509" s="43"/>
-    </row>
-    <row r="510" spans="7:9">
-      <c r="G510" s="41"/>
-      <c r="H510" s="42"/>
+      <c r="J507" s="40">
+        <v>282</v>
+      </c>
+      <c r="K507" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L507" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="R507" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V507" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="2:22">
+      <c r="B508" s="35" t="s">
+        <v>530</v>
+      </c>
+      <c r="G508" s="41" t="s">
+        <v>531</v>
+      </c>
+      <c r="H508" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I508" s="43" t="s">
+        <v>533</v>
+      </c>
+      <c r="J508" s="40">
+        <v>468</v>
+      </c>
+      <c r="K508" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L508" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R508" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V508" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="2:22">
+      <c r="B509" s="35" t="s">
+        <v>534</v>
+      </c>
+      <c r="G509" s="41" t="s">
+        <v>535</v>
+      </c>
+      <c r="H509" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="I509" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="J509" s="40">
+        <v>129</v>
+      </c>
+      <c r="K509" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L509" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="R509" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V509" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="2:22">
+      <c r="B510" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="G510" s="41" t="s">
+        <v>531</v>
+      </c>
+      <c r="H510" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="I510" s="43"/>
-    </row>
-    <row r="514" spans="7:12">
-      <c r="G514" s="41"/>
-      <c r="H514" s="42"/>
-      <c r="I514" s="43"/>
-      <c r="J514" s="44"/>
-      <c r="K514" s="42"/>
-      <c r="L514" s="42"/>
-    </row>
-    <row r="515" spans="7:12">
-      <c r="G515" s="41"/>
-      <c r="H515" s="42"/>
-      <c r="I515" s="43"/>
-      <c r="J515" s="44"/>
-      <c r="K515" s="42"/>
-      <c r="L515" s="42"/>
-    </row>
-    <row r="516" spans="7:12">
-      <c r="G516" s="41"/>
-      <c r="H516" s="42"/>
-      <c r="I516" s="43"/>
+      <c r="J510" s="40">
+        <v>163</v>
+      </c>
+      <c r="K510" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L510" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R510" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V510" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="2:22">
+      <c r="B511" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="G511" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="H511" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I511" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="J511" s="40">
+        <v>227</v>
+      </c>
+      <c r="K511" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L511" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="R511" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V511" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="2:22">
+      <c r="B512" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="G512" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="H512" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I512" s="34" t="s">
+        <v>532</v>
+      </c>
+      <c r="J512" s="40">
+        <v>249</v>
+      </c>
+      <c r="K512" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L512" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R512" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V512" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="2:22">
+      <c r="B513" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="G513" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="H513" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J513" s="40">
+        <v>282</v>
+      </c>
+      <c r="K513" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L513" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="R513" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V513" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="2:22">
+      <c r="B514" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="G514" s="41" t="s">
+        <v>531</v>
+      </c>
+      <c r="H514" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I514" s="43" t="s">
+        <v>533</v>
+      </c>
+      <c r="J514" s="44">
+        <v>468</v>
+      </c>
+      <c r="K514" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="L514" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="R514" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V514" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="2:22">
+      <c r="B515" s="35" t="s">
+        <v>537</v>
+      </c>
+      <c r="G515" s="41" t="s">
+        <v>535</v>
+      </c>
+      <c r="H515" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="I515" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="J515" s="44">
+        <v>129</v>
+      </c>
+      <c r="K515" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="L515" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="R515" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V515" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="2:22">
+      <c r="B516" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="G516" s="41" t="s">
+        <v>539</v>
+      </c>
+      <c r="H516" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="I516" s="43" t="s">
+        <v>322</v>
+      </c>
+      <c r="J516" s="40">
+        <v>116</v>
+      </c>
+      <c r="K516" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L516" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="R516" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V516" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="2:22">
+      <c r="B517" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="G517" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H517" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J517" s="40">
+        <v>169</v>
+      </c>
+      <c r="K517" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L517" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R517" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V517" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="2:22">
+      <c r="B518" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="G518" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H518" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I518" s="34" t="s">
+        <v>540</v>
+      </c>
+      <c r="J518" s="40">
+        <v>230</v>
+      </c>
+      <c r="K518" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L518" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R518" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V518" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" spans="2:22">
+      <c r="B519" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="G519" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H519" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I519" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="J519" s="40">
+        <v>234</v>
+      </c>
+      <c r="K519" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L519" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R519" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V519" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" spans="2:22">
+      <c r="B520" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="G520" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H520" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I520" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="J520" s="40">
+        <v>289</v>
+      </c>
+      <c r="K520" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L520" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R520" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V520" s="138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" spans="2:22">
+      <c r="B521" s="35" t="s">
+        <v>541</v>
+      </c>
+      <c r="G521" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="H521" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J521" s="40">
+        <v>194</v>
+      </c>
+      <c r="K521" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="L521" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R521" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V521" s="138" t="b">
+        <f t="shared" ref="V521:V541" si="9">AND(ISBLANK(M521),ISBLANK(N521),ISBLANK(O521),ISBLANK(P521),ISBLANK(Q521))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="2:22">
+      <c r="B522" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="G522" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H522" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I522" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="J522" s="40">
+        <v>116</v>
+      </c>
+      <c r="K522" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L522" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="R522" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V522" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="2:22">
+      <c r="B523" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="G523" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H523" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J523" s="40">
+        <v>169</v>
+      </c>
+      <c r="K523" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L523" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R523" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V523" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="2:22">
+      <c r="B524" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="G524" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H524" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I524" s="34" t="s">
+        <v>540</v>
+      </c>
+      <c r="J524" s="40">
+        <v>230</v>
+      </c>
+      <c r="K524" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L524" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R524" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V524" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" spans="2:22">
+      <c r="B525" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="G525" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H525" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I525" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="J525" s="40">
+        <v>234</v>
+      </c>
+      <c r="K525" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L525" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R525" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V525" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" spans="2:22">
+      <c r="B526" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="G526" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="H526" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I526" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="J526" s="40">
+        <v>289</v>
+      </c>
+      <c r="K526" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L526" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R526" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="V526" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" spans="2:22">
+      <c r="B527" s="35" t="s">
+        <v>543</v>
+      </c>
+      <c r="G527" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H527" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J527" s="40">
+        <v>2</v>
+      </c>
+      <c r="K527" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L527" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R527" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V527" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="2:22">
+      <c r="B528" s="35" t="s">
+        <v>543</v>
+      </c>
+      <c r="G528" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H528" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J528" s="40">
+        <v>282</v>
+      </c>
+      <c r="K528" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L528" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R528" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V528" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="2:22">
+      <c r="B529" s="35" t="s">
+        <v>544</v>
+      </c>
+      <c r="G529" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H529" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J529" s="40">
+        <v>2</v>
+      </c>
+      <c r="K529" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L529" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R529" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V529" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="530" spans="2:22">
+      <c r="B530" s="35" t="s">
+        <v>544</v>
+      </c>
+      <c r="G530" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H530" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J530" s="40">
+        <v>282</v>
+      </c>
+      <c r="K530" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L530" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R530" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V530" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" spans="2:22">
+      <c r="B531" s="35" t="s">
+        <v>545</v>
+      </c>
+      <c r="G531" s="21" t="s">
+        <v>500</v>
+      </c>
+      <c r="H531" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I531" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="J531" s="40">
+        <v>144</v>
+      </c>
+      <c r="K531" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L531" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="R531" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V531" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" spans="2:22">
+      <c r="B532" s="35" t="s">
+        <v>546</v>
+      </c>
+      <c r="G532" s="21" t="s">
+        <v>500</v>
+      </c>
+      <c r="H532" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I532" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="J532" s="40">
+        <v>144</v>
+      </c>
+      <c r="K532" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L532" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="R532" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V532" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533" spans="2:22">
+      <c r="B533" s="35" t="s">
+        <v>547</v>
+      </c>
+      <c r="G533" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H533" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J533" s="40">
+        <v>2</v>
+      </c>
+      <c r="K533" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L533" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R533" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V533" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" spans="2:22">
+      <c r="B534" s="35" t="s">
+        <v>547</v>
+      </c>
+      <c r="G534" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H534" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J534" s="40">
+        <v>282</v>
+      </c>
+      <c r="K534" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L534" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R534" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V534" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" spans="2:22">
+      <c r="B535" s="35" t="s">
+        <v>548</v>
+      </c>
+      <c r="G535" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H535" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J535" s="40">
+        <v>2</v>
+      </c>
+      <c r="K535" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L535" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R535" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V535" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" spans="2:22">
+      <c r="B536" s="35" t="s">
+        <v>548</v>
+      </c>
+      <c r="G536" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H536" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J536" s="40">
+        <v>282</v>
+      </c>
+      <c r="K536" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L536" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R536" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V536" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537" spans="2:22">
+      <c r="B537" s="35" t="s">
+        <v>549</v>
+      </c>
+      <c r="G537" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H537" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J537" s="40">
+        <v>2</v>
+      </c>
+      <c r="K537" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L537" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R537" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V537" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" spans="2:22">
+      <c r="B538" s="35" t="s">
+        <v>549</v>
+      </c>
+      <c r="G538" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H538" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J538" s="40">
+        <v>282</v>
+      </c>
+      <c r="K538" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L538" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R538" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V538" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="539" spans="2:22">
+      <c r="B539" s="35" t="s">
+        <v>550</v>
+      </c>
+      <c r="G539" s="21" t="s">
+        <v>551</v>
+      </c>
+      <c r="H539" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I539" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="J539" s="40">
+        <v>66</v>
+      </c>
+      <c r="K539" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L539" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="R539" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V539" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" spans="2:22">
+      <c r="B540" s="35" t="s">
+        <v>550</v>
+      </c>
+      <c r="G540" s="21" t="s">
+        <v>551</v>
+      </c>
+      <c r="H540" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I540" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="J540" s="40">
+        <v>304</v>
+      </c>
+      <c r="K540" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L540" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="R540" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V540" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="2:22">
+      <c r="B541" s="35" t="s">
+        <v>552</v>
+      </c>
+      <c r="G541" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H541" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J541" s="40">
+        <v>154</v>
+      </c>
+      <c r="K541" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L541" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R541" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="V541" s="138" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="593" spans="7:13">
       <c r="G593" s="41"/>
@@ -28010,12 +29330,12 @@
   <dataConsolidate/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="V1:V101 V103:V171 V173:V1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V172">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44421,12 +45741,12 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="V165:V1048576 V95:V163 V1:V93">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V164">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46558,7 +47878,7 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48458,7 +49778,7 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FIX: corrected wrong class annotation
</commit_message>
<xml_diff>
--- a/structure_data/construct_data/Stabilising_Mutations_In_Xtal_Constructs.xlsx
+++ b/structure_data/construct_data/Stabilising_Mutations_In_Xtal_Constructs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rwf545/Dropbox (GloriamGroup)/1.GPCRdb/GPCRdb_Proj_Construct_db/Annotation/Annotated_Mutations-David/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/tmp/gpcrdb_data/structure_data/construct_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B5BAE0-6061-1E4F-87FF-5D361CC4E58E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA42D7C-940B-FD43-8604-E3E801EBDD69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mutation_Data" sheetId="1" r:id="rId1"/>
@@ -7433,8 +7433,8 @@
   <dimension ref="A1:X673"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F449" sqref="F449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21629,7 +21629,7 @@
         <v>203</v>
       </c>
       <c r="V386" s="36" t="b">
-        <f t="shared" ref="V386:V449" si="6">AND(ISBLANK(M386),ISBLANK(N386),ISBLANK(O386),ISBLANK(P386),ISBLANK(Q386))</f>
+        <f t="shared" ref="V386:V453" si="6">AND(ISBLANK(M386),ISBLANK(N386),ISBLANK(O386),ISBLANK(P386),ISBLANK(Q386))</f>
         <v>0</v>
       </c>
     </row>
@@ -23818,90 +23818,134 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A446" s="36"/>
+      <c r="B446" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="C446" s="36"/>
       <c r="D446" s="18" t="s">
-        <v>90</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E446" s="36"/>
+      <c r="F446" s="36"/>
       <c r="G446" s="20" t="s">
-        <v>160</v>
+        <v>483</v>
       </c>
       <c r="H446" s="18" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="I446" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="J446" s="61">
-        <v>120</v>
+        <v>484</v>
+      </c>
+      <c r="J446" s="139">
+        <v>83</v>
       </c>
       <c r="K446" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="L446" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M446" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="N446" s="37"/>
+      <c r="O446" s="36"/>
+      <c r="P446" s="36"/>
+      <c r="Q446" s="36"/>
+      <c r="R446" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="S446" s="36"/>
+      <c r="T446" s="36"/>
+      <c r="U446" s="36"/>
+      <c r="V446" s="36" t="b">
+        <f>AND(ISBLANK(M446),ISBLANK(N446),ISBLANK(O446),ISBLANK(P446),ISBLANK(Q446))</f>
+        <v>0</v>
+      </c>
+      <c r="W446" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="X446" s="36"/>
+    </row>
+    <row r="447" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A447" s="36"/>
+      <c r="B447" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="C447" s="36"/>
+      <c r="D447" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E447" s="36"/>
+      <c r="F447" s="36"/>
+      <c r="G447" s="20" t="s">
+        <v>483</v>
+      </c>
+      <c r="H447" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I447" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="J447" s="139">
+        <v>88</v>
+      </c>
+      <c r="K447" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L447" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M447" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="N447" s="37"/>
+      <c r="O447" s="36"/>
+      <c r="P447" s="36"/>
+      <c r="Q447" s="36"/>
+      <c r="R447" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="S447" s="36"/>
+      <c r="T447" s="36"/>
+      <c r="U447" s="36"/>
+      <c r="V447" s="36" t="b">
+        <f>AND(ISBLANK(M447),ISBLANK(N447),ISBLANK(O447),ISBLANK(P447),ISBLANK(Q447))</f>
+        <v>0</v>
+      </c>
+      <c r="W447" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="X447" s="36"/>
+    </row>
+    <row r="448" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A448" s="36"/>
+      <c r="B448" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="C448" s="36"/>
+      <c r="D448" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E448" s="36"/>
+      <c r="F448" s="36"/>
+      <c r="G448" s="20" t="s">
+        <v>483</v>
+      </c>
+      <c r="H448" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I448" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="J448" s="139">
+        <v>212</v>
+      </c>
+      <c r="K448" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="L446" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M446" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N446" s="37"/>
-      <c r="V446" s="36" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="447" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D447" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="G447" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H447" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="I447" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="J447" s="61">
-        <v>144</v>
-      </c>
-      <c r="K447" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="L447" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M447" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N447" s="37"/>
-      <c r="V447" s="36" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="448" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B448" s="36" t="s">
-        <v>397</v>
-      </c>
-      <c r="D448" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="G448" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H448" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="I448" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="J448" s="61">
-        <v>156</v>
-      </c>
-      <c r="K448" s="18" t="s">
-        <v>46</v>
-      </c>
       <c r="L448" s="18" t="s">
         <v>39</v>
       </c>
@@ -23909,29 +23953,44 @@
         <v>205</v>
       </c>
       <c r="N448" s="37"/>
+      <c r="O448" s="36"/>
+      <c r="P448" s="36"/>
+      <c r="Q448" s="36"/>
+      <c r="R448" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="S448" s="36"/>
+      <c r="T448" s="36"/>
+      <c r="U448" s="36"/>
       <c r="V448" s="36" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="449" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+        <f>AND(ISBLANK(M448),ISBLANK(N448),ISBLANK(O448),ISBLANK(P448),ISBLANK(Q448))</f>
+        <v>0</v>
+      </c>
+      <c r="W448" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="X448" s="36"/>
+    </row>
+    <row r="449" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A449" s="36"/>
       <c r="B449" s="36" t="s">
-        <v>397</v>
-      </c>
+        <v>482</v>
+      </c>
+      <c r="C449" s="36"/>
       <c r="D449" s="18" t="s">
-        <v>410</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E449" s="36"/>
+      <c r="F449" s="36"/>
       <c r="G449" s="20" t="s">
-        <v>160</v>
+        <v>483</v>
       </c>
       <c r="H449" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="I449" s="39" t="s">
-        <v>310</v>
-      </c>
-      <c r="J449" s="61">
-        <v>160</v>
+        <v>241</v>
+      </c>
+      <c r="I449" s="39"/>
+      <c r="J449" s="139">
+        <v>309</v>
       </c>
       <c r="K449" s="18" t="s">
         <v>47</v>
@@ -23943,15 +24002,25 @@
         <v>205</v>
       </c>
       <c r="N449" s="37"/>
+      <c r="O449" s="36"/>
+      <c r="P449" s="36"/>
+      <c r="Q449" s="36"/>
+      <c r="R449" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="S449" s="36"/>
+      <c r="T449" s="36"/>
+      <c r="U449" s="36"/>
       <c r="V449" s="36" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="450" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B450" s="36" t="s">
-        <v>397</v>
-      </c>
+        <f>AND(ISBLANK(M449),ISBLANK(N449),ISBLANK(O449),ISBLANK(P449),ISBLANK(Q449))</f>
+        <v>0</v>
+      </c>
+      <c r="W449" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="X449" s="36"/>
+    </row>
+    <row r="450" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D450" s="18" t="s">
         <v>410</v>
       </c>
@@ -23959,16 +24028,16 @@
         <v>160</v>
       </c>
       <c r="H450" s="18" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="I450" s="39" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="J450" s="61">
-        <v>228</v>
+        <v>120</v>
       </c>
       <c r="K450" s="18" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="L450" s="18" t="s">
         <v>39</v>
@@ -23978,14 +24047,11 @@
       </c>
       <c r="N450" s="37"/>
       <c r="V450" s="36" t="b">
-        <f t="shared" ref="V450:V513" si="7">AND(ISBLANK(M450),ISBLANK(N450),ISBLANK(O450),ISBLANK(P450),ISBLANK(Q450))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="451" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B451" s="36" t="s">
-        <v>397</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D451" s="18" t="s">
         <v>410</v>
       </c>
@@ -23993,16 +24059,16 @@
         <v>160</v>
       </c>
       <c r="H451" s="18" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="I451" s="39" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="J451" s="61">
-        <v>260</v>
+        <v>144</v>
       </c>
       <c r="K451" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L451" s="18" t="s">
         <v>39</v>
@@ -24010,13 +24076,13 @@
       <c r="M451" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="N451" s="64"/>
+      <c r="N451" s="37"/>
       <c r="V451" s="36" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="452" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B452" s="36" t="s">
         <v>397</v>
       </c>
@@ -24027,16 +24093,16 @@
         <v>160</v>
       </c>
       <c r="H452" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I452" s="39" t="s">
-        <v>183</v>
+        <v>280</v>
       </c>
       <c r="J452" s="61">
-        <v>277</v>
+        <v>156</v>
       </c>
       <c r="K452" s="18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L452" s="18" t="s">
         <v>39</v>
@@ -24046,11 +24112,11 @@
       </c>
       <c r="N452" s="37"/>
       <c r="V452" s="36" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="453" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B453" s="36" t="s">
         <v>397</v>
       </c>
@@ -24061,16 +24127,16 @@
         <v>160</v>
       </c>
       <c r="H453" s="18" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I453" s="39" t="s">
-        <v>188</v>
+        <v>310</v>
       </c>
       <c r="J453" s="61">
-        <v>309</v>
+        <v>160</v>
       </c>
       <c r="K453" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L453" s="18" t="s">
         <v>39</v>
@@ -24080,11 +24146,11 @@
       </c>
       <c r="N453" s="37"/>
       <c r="V453" s="36" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="454" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B454" s="36" t="s">
         <v>397</v>
       </c>
@@ -24095,16 +24161,16 @@
         <v>160</v>
       </c>
       <c r="H454" s="18" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="I454" s="39" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="J454" s="61">
-        <v>330</v>
+        <v>228</v>
       </c>
       <c r="K454" s="18" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="L454" s="18" t="s">
         <v>39</v>
@@ -24114,11 +24180,11 @@
       </c>
       <c r="N454" s="37"/>
       <c r="V454" s="36" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="455" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="V454:V517" si="7">AND(ISBLANK(M454),ISBLANK(N454),ISBLANK(O454),ISBLANK(P454),ISBLANK(Q454))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B455" s="36" t="s">
         <v>397</v>
       </c>
@@ -24129,16 +24195,16 @@
         <v>160</v>
       </c>
       <c r="H455" s="18" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="I455" s="39" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="J455" s="61">
-        <v>349</v>
+        <v>260</v>
       </c>
       <c r="K455" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L455" s="18" t="s">
         <v>39</v>
@@ -24146,13 +24212,13 @@
       <c r="M455" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="N455" s="37"/>
+      <c r="N455" s="64"/>
       <c r="V455" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B456" s="36" t="s">
         <v>397</v>
       </c>
@@ -24163,16 +24229,16 @@
         <v>160</v>
       </c>
       <c r="H456" s="18" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="I456" s="39" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="J456" s="61">
-        <v>363</v>
+        <v>277</v>
       </c>
       <c r="K456" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L456" s="18" t="s">
         <v>39</v>
@@ -24186,140 +24252,132 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B457" s="36" t="s">
-        <v>287</v>
+        <v>397</v>
       </c>
       <c r="D457" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G457" s="20" t="s">
-        <v>288</v>
+        <v>160</v>
       </c>
       <c r="H457" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I457" s="39"/>
+        <v>92</v>
+      </c>
+      <c r="I457" s="39" t="s">
+        <v>188</v>
+      </c>
       <c r="J457" s="61">
-        <v>106</v>
+        <v>309</v>
       </c>
       <c r="K457" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L457" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M457" s="53"/>
+      <c r="M457" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N457" s="37"/>
-      <c r="Q457" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="R457" s="36" t="s">
-        <v>226</v>
-      </c>
       <c r="V457" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B458" s="36" t="s">
-        <v>287</v>
+        <v>397</v>
       </c>
       <c r="D458" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G458" s="20" t="s">
-        <v>288</v>
+        <v>160</v>
       </c>
       <c r="H458" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I458" s="39"/>
+        <v>92</v>
+      </c>
+      <c r="I458" s="39" t="s">
+        <v>192</v>
+      </c>
       <c r="J458" s="61">
-        <v>112</v>
+        <v>330</v>
       </c>
       <c r="K458" s="18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L458" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="M458" s="68"/>
+        <v>39</v>
+      </c>
+      <c r="M458" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N458" s="37"/>
-      <c r="Q458" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="R458" s="36" t="s">
-        <v>226</v>
-      </c>
       <c r="V458" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B459" s="36" t="s">
-        <v>287</v>
+        <v>397</v>
       </c>
       <c r="D459" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G459" s="20" t="s">
-        <v>288</v>
+        <v>160</v>
       </c>
       <c r="H459" s="18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I459" s="39" t="s">
-        <v>289</v>
+        <v>195</v>
       </c>
       <c r="J459" s="61">
-        <v>140</v>
+        <v>349</v>
       </c>
       <c r="K459" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L459" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="M459" s="53"/>
+        <v>39</v>
+      </c>
+      <c r="M459" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N459" s="37"/>
-      <c r="Q459" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="R459" s="36" t="s">
-        <v>226</v>
-      </c>
       <c r="V459" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B460" s="36" t="s">
-        <v>290</v>
+        <v>397</v>
       </c>
       <c r="D460" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G460" s="20" t="s">
-        <v>291</v>
+        <v>160</v>
       </c>
       <c r="H460" s="18" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="I460" s="39" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="J460" s="61">
-        <v>193</v>
+        <v>363</v>
       </c>
       <c r="K460" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L460" s="18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="M460" s="53" t="s">
         <v>205</v>
@@ -24330,111 +24388,119 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B461" s="36" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D461" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G461" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H461" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="I461" s="39" t="s">
-        <v>100</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="I461" s="39"/>
       <c r="J461" s="61">
-        <v>193</v>
+        <v>106</v>
       </c>
       <c r="K461" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L461" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="M461" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="M461" s="53"/>
       <c r="N461" s="37"/>
+      <c r="Q461" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="R461" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="V461" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B462" s="36" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D462" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G462" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H462" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="I462" s="39" t="s">
-        <v>293</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="I462" s="39"/>
       <c r="J462" s="61">
-        <v>196</v>
+        <v>112</v>
       </c>
       <c r="K462" s="18" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="L462" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="M462" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="M462" s="68"/>
       <c r="N462" s="37"/>
+      <c r="Q462" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="R462" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="V462" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B463" s="36" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D463" s="18" t="s">
         <v>410</v>
       </c>
       <c r="G463" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H463" s="18" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="I463" s="39" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J463" s="61">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="K463" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="L463" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="M463" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="M463" s="53"/>
       <c r="N463" s="37"/>
+      <c r="Q463" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="R463" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="V463" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B464" s="36" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D464" s="18" t="s">
         <v>410</v>
@@ -24443,17 +24509,19 @@
         <v>291</v>
       </c>
       <c r="H464" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="I464" s="39"/>
+        <v>99</v>
+      </c>
+      <c r="I464" s="39" t="s">
+        <v>100</v>
+      </c>
       <c r="J464" s="61">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="K464" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L464" s="18" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="M464" s="53" t="s">
         <v>205</v>
@@ -24466,7 +24534,7 @@
     </row>
     <row r="465" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B465" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D465" s="18" t="s">
         <v>410</v>
@@ -24475,17 +24543,19 @@
         <v>291</v>
       </c>
       <c r="H465" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="I465" s="39"/>
+        <v>99</v>
+      </c>
+      <c r="I465" s="39" t="s">
+        <v>100</v>
+      </c>
       <c r="J465" s="61">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="K465" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L465" s="18" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="M465" s="53" t="s">
         <v>205</v>
@@ -24498,7 +24568,7 @@
     </row>
     <row r="466" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B466" s="36" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D466" s="18" t="s">
         <v>410</v>
@@ -24507,17 +24577,19 @@
         <v>291</v>
       </c>
       <c r="H466" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="I466" s="39"/>
+        <v>99</v>
+      </c>
+      <c r="I466" s="39" t="s">
+        <v>293</v>
+      </c>
       <c r="J466" s="61">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="K466" s="18" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L466" s="18" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="M466" s="53" t="s">
         <v>205</v>
@@ -24530,7 +24602,7 @@
     </row>
     <row r="467" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B467" s="36" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D467" s="18" t="s">
         <v>410</v>
@@ -24539,19 +24611,19 @@
         <v>291</v>
       </c>
       <c r="H467" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I467" s="39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J467" s="61">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="K467" s="18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L467" s="18" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M467" s="53" t="s">
         <v>205</v>
@@ -24564,7 +24636,7 @@
     </row>
     <row r="468" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B468" s="36" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D468" s="18" t="s">
         <v>410</v>
@@ -24573,19 +24645,17 @@
         <v>291</v>
       </c>
       <c r="H468" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I468" s="39" t="s">
-        <v>295</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I468" s="39"/>
       <c r="J468" s="61">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="K468" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L468" s="18" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="M468" s="53" t="s">
         <v>205</v>
@@ -24607,19 +24677,17 @@
         <v>291</v>
       </c>
       <c r="H469" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I469" s="39" t="s">
-        <v>296</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I469" s="39"/>
       <c r="J469" s="61">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="K469" s="18" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="L469" s="18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M469" s="53" t="s">
         <v>205</v>
@@ -24632,7 +24700,7 @@
     </row>
     <row r="470" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B470" s="36" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D470" s="18" t="s">
         <v>410</v>
@@ -24641,27 +24709,22 @@
         <v>291</v>
       </c>
       <c r="H470" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I470" s="39" t="s">
-        <v>297</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I470" s="39"/>
       <c r="J470" s="61">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="K470" s="18" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="L470" s="18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M470" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N470" s="37"/>
-      <c r="U470" s="36" t="s">
-        <v>332</v>
-      </c>
       <c r="V470" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -24669,7 +24732,7 @@
     </row>
     <row r="471" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B471" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D471" s="18" t="s">
         <v>410</v>
@@ -24681,24 +24744,21 @@
         <v>95</v>
       </c>
       <c r="I471" s="39" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J471" s="61">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K471" s="18" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="L471" s="18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="M471" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N471" s="37"/>
-      <c r="U471" s="36" t="s">
-        <v>332</v>
-      </c>
       <c r="V471" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -24706,7 +24766,7 @@
     </row>
     <row r="472" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B472" s="36" t="s">
-        <v>408</v>
+        <v>292</v>
       </c>
       <c r="D472" s="18" t="s">
         <v>410</v>
@@ -24718,25 +24778,21 @@
         <v>95</v>
       </c>
       <c r="I472" s="39" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J472" s="61">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K472" s="18" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="L472" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="M472" s="53"/>
+        <v>39</v>
+      </c>
+      <c r="M472" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N472" s="37"/>
-      <c r="Q472" s="36" t="s">
-        <v>336</v>
-      </c>
-      <c r="R472" s="36" t="s">
-        <v>409</v>
-      </c>
       <c r="V472" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -24744,7 +24800,7 @@
     </row>
     <row r="473" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B473" s="36" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D473" s="18" t="s">
         <v>410</v>
@@ -24753,26 +24809,24 @@
         <v>291</v>
       </c>
       <c r="H473" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I473" s="39"/>
+        <v>95</v>
+      </c>
+      <c r="I473" s="39" t="s">
+        <v>296</v>
+      </c>
       <c r="J473" s="61">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="K473" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L473" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M473" s="53"/>
+        <v>44</v>
+      </c>
+      <c r="M473" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N473" s="37"/>
-      <c r="Q473" s="36" t="s">
-        <v>329</v>
-      </c>
-      <c r="R473" s="36" t="s">
-        <v>226</v>
-      </c>
       <c r="V473" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -24780,7 +24834,7 @@
     </row>
     <row r="474" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B474" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D474" s="18" t="s">
         <v>410</v>
@@ -24789,25 +24843,26 @@
         <v>291</v>
       </c>
       <c r="H474" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I474" s="39"/>
+        <v>95</v>
+      </c>
+      <c r="I474" s="39" t="s">
+        <v>297</v>
+      </c>
       <c r="J474" s="61">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="K474" s="18" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="L474" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M474" s="53"/>
+        <v>49</v>
+      </c>
+      <c r="M474" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N474" s="37"/>
-      <c r="Q474" s="36" t="s">
-        <v>329</v>
-      </c>
-      <c r="R474" s="36" t="s">
-        <v>226</v>
+      <c r="U474" s="36" t="s">
+        <v>332</v>
       </c>
       <c r="V474" s="36" t="b">
         <f t="shared" si="7"/>
@@ -24816,7 +24871,7 @@
     </row>
     <row r="475" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B475" s="36" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D475" s="18" t="s">
         <v>410</v>
@@ -24825,25 +24880,26 @@
         <v>291</v>
       </c>
       <c r="H475" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I475" s="39"/>
+        <v>95</v>
+      </c>
+      <c r="I475" s="39" t="s">
+        <v>297</v>
+      </c>
       <c r="J475" s="61">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="K475" s="18" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L475" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="M475" s="53"/>
+        <v>49</v>
+      </c>
+      <c r="M475" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N475" s="37"/>
-      <c r="Q475" s="36" t="s">
-        <v>329</v>
-      </c>
-      <c r="R475" s="36" t="s">
-        <v>226</v>
+      <c r="U475" s="36" t="s">
+        <v>332</v>
       </c>
       <c r="V475" s="36" t="b">
         <f t="shared" si="7"/>
@@ -24852,7 +24908,7 @@
     </row>
     <row r="476" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B476" s="36" t="s">
-        <v>292</v>
+        <v>408</v>
       </c>
       <c r="D476" s="18" t="s">
         <v>410</v>
@@ -24861,25 +24917,27 @@
         <v>291</v>
       </c>
       <c r="H476" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I476" s="39"/>
+        <v>95</v>
+      </c>
+      <c r="I476" s="39" t="s">
+        <v>297</v>
+      </c>
       <c r="J476" s="61">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="K476" s="18" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L476" s="18" t="s">
-        <v>42</v>
+        <v>249</v>
       </c>
       <c r="M476" s="53"/>
       <c r="N476" s="37"/>
       <c r="Q476" s="36" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="R476" s="36" t="s">
-        <v>226</v>
+        <v>409</v>
       </c>
       <c r="V476" s="36" t="b">
         <f t="shared" si="7"/>
@@ -24888,7 +24946,7 @@
     </row>
     <row r="477" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B477" s="36" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D477" s="18" t="s">
         <v>410</v>
@@ -24901,23 +24959,21 @@
       </c>
       <c r="I477" s="39"/>
       <c r="J477" s="61">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K477" s="18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L477" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="M477" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M477" s="53"/>
       <c r="N477" s="37"/>
       <c r="Q477" s="36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R477" s="36" t="s">
-        <v>298</v>
+        <v>226</v>
       </c>
       <c r="V477" s="36" t="b">
         <f t="shared" si="7"/>
@@ -24926,7 +24982,7 @@
     </row>
     <row r="478" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B478" s="36" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D478" s="18" t="s">
         <v>410</v>
@@ -24939,19 +24995,22 @@
       </c>
       <c r="I478" s="39"/>
       <c r="J478" s="61">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K478" s="18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L478" s="18" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="M478" s="53"/>
       <c r="N478" s="37"/>
       <c r="Q478" s="36" t="s">
         <v>329</v>
       </c>
+      <c r="R478" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="V478" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -24959,7 +25018,7 @@
     </row>
     <row r="479" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B479" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D479" s="18" t="s">
         <v>410</v>
@@ -24972,19 +25031,22 @@
       </c>
       <c r="I479" s="39"/>
       <c r="J479" s="61">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K479" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L479" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M479" s="53"/>
       <c r="N479" s="37"/>
       <c r="Q479" s="36" t="s">
         <v>329</v>
       </c>
+      <c r="R479" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="V479" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -24992,7 +25054,7 @@
     </row>
     <row r="480" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B480" s="36" t="s">
-        <v>498</v>
+        <v>292</v>
       </c>
       <c r="D480" s="18" t="s">
         <v>410</v>
@@ -25004,20 +25066,23 @@
         <v>117</v>
       </c>
       <c r="I480" s="39"/>
-      <c r="J480" s="61" t="s">
-        <v>457</v>
+      <c r="J480" s="61">
+        <v>259</v>
       </c>
       <c r="K480" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L480" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M480" s="53"/>
       <c r="N480" s="37"/>
       <c r="Q480" s="36" t="s">
         <v>329</v>
       </c>
+      <c r="R480" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="V480" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -25025,7 +25090,7 @@
     </row>
     <row r="481" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B481" s="36" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D481" s="18" t="s">
         <v>410</v>
@@ -25034,24 +25099,28 @@
         <v>291</v>
       </c>
       <c r="H481" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I481" s="39" t="s">
-        <v>299</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="I481" s="39"/>
       <c r="J481" s="61">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K481" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L481" s="18" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M481" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N481" s="37"/>
+      <c r="Q481" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="R481" s="36" t="s">
+        <v>298</v>
+      </c>
       <c r="V481" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -25059,7 +25128,7 @@
     </row>
     <row r="482" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B482" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D482" s="18" t="s">
         <v>410</v>
@@ -25068,24 +25137,23 @@
         <v>291</v>
       </c>
       <c r="H482" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I482" s="39" t="s">
-        <v>299</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="I482" s="39"/>
       <c r="J482" s="61">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K482" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L482" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M482" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M482" s="53"/>
       <c r="N482" s="37"/>
+      <c r="Q482" s="36" t="s">
+        <v>329</v>
+      </c>
       <c r="V482" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -25093,7 +25161,7 @@
     </row>
     <row r="483" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B483" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D483" s="18" t="s">
         <v>410</v>
@@ -25102,22 +25170,23 @@
         <v>291</v>
       </c>
       <c r="H483" s="18" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I483" s="39"/>
       <c r="J483" s="61">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="K483" s="18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L483" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M483" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M483" s="53"/>
       <c r="N483" s="37"/>
+      <c r="Q483" s="36" t="s">
+        <v>329</v>
+      </c>
       <c r="V483" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -25125,7 +25194,7 @@
     </row>
     <row r="484" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B484" s="36" t="s">
-        <v>294</v>
+        <v>498</v>
       </c>
       <c r="D484" s="18" t="s">
         <v>410</v>
@@ -25134,24 +25203,23 @@
         <v>291</v>
       </c>
       <c r="H484" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="I484" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="J484" s="61">
-        <v>298</v>
+        <v>117</v>
+      </c>
+      <c r="I484" s="39"/>
+      <c r="J484" s="61" t="s">
+        <v>457</v>
       </c>
       <c r="K484" s="18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="L484" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M484" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M484" s="53"/>
       <c r="N484" s="37"/>
+      <c r="Q484" s="36" t="s">
+        <v>329</v>
+      </c>
       <c r="V484" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -25168,19 +25236,19 @@
         <v>291</v>
       </c>
       <c r="H485" s="18" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="I485" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J485" s="61">
-        <v>317</v>
+        <v>271</v>
       </c>
       <c r="K485" s="18" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L485" s="18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="M485" s="53" t="s">
         <v>205</v>
@@ -25202,19 +25270,19 @@
         <v>291</v>
       </c>
       <c r="H486" s="18" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="I486" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J486" s="61">
-        <v>317</v>
+        <v>271</v>
       </c>
       <c r="K486" s="18" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L486" s="18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="M486" s="53" t="s">
         <v>205</v>
@@ -25227,7 +25295,7 @@
     </row>
     <row r="487" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B487" s="36" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D487" s="18" t="s">
         <v>410</v>
@@ -25236,19 +25304,17 @@
         <v>291</v>
       </c>
       <c r="H487" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="I487" s="39" t="s">
-        <v>301</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="I487" s="39"/>
       <c r="J487" s="61">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="K487" s="18" t="s">
         <v>38</v>
       </c>
       <c r="L487" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M487" s="53" t="s">
         <v>205</v>
@@ -25261,7 +25327,7 @@
     </row>
     <row r="488" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B488" s="36" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D488" s="18" t="s">
         <v>410</v>
@@ -25270,19 +25336,19 @@
         <v>291</v>
       </c>
       <c r="H488" s="18" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I488" s="39" t="s">
-        <v>301</v>
+        <v>180</v>
       </c>
       <c r="J488" s="61">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="K488" s="18" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="L488" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M488" s="53" t="s">
         <v>205</v>
@@ -25295,7 +25361,7 @@
     </row>
     <row r="489" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B489" s="36" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D489" s="18" t="s">
         <v>410</v>
@@ -25307,16 +25373,16 @@
         <v>102</v>
       </c>
       <c r="I489" s="39" t="s">
-        <v>148</v>
+        <v>300</v>
       </c>
       <c r="J489" s="61">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="K489" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L489" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="L489" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="M489" s="53" t="s">
         <v>205</v>
@@ -25329,7 +25395,7 @@
     </row>
     <row r="490" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B490" s="36" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D490" s="18" t="s">
         <v>410</v>
@@ -25338,19 +25404,19 @@
         <v>291</v>
       </c>
       <c r="H490" s="18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="I490" s="39" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="J490" s="61">
-        <v>346</v>
+        <v>317</v>
       </c>
       <c r="K490" s="18" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L490" s="18" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="M490" s="53" t="s">
         <v>205</v>
@@ -25363,7 +25429,7 @@
     </row>
     <row r="491" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B491" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D491" s="18" t="s">
         <v>410</v>
@@ -25372,19 +25438,19 @@
         <v>291</v>
       </c>
       <c r="H491" s="18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="I491" s="39" t="s">
-        <v>188</v>
+        <v>301</v>
       </c>
       <c r="J491" s="61">
-        <v>346</v>
+        <v>318</v>
       </c>
       <c r="K491" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="L491" s="18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M491" s="53" t="s">
         <v>205</v>
@@ -25397,7 +25463,7 @@
     </row>
     <row r="492" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B492" s="36" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D492" s="18" t="s">
         <v>410</v>
@@ -25406,19 +25472,19 @@
         <v>291</v>
       </c>
       <c r="H492" s="18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="I492" s="39" t="s">
-        <v>257</v>
+        <v>301</v>
       </c>
       <c r="J492" s="61">
-        <v>347</v>
+        <v>318</v>
       </c>
       <c r="K492" s="18" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="L492" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M492" s="53" t="s">
         <v>205</v>
@@ -25431,7 +25497,7 @@
     </row>
     <row r="493" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B493" s="36" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D493" s="18" t="s">
         <v>410</v>
@@ -25440,19 +25506,19 @@
         <v>291</v>
       </c>
       <c r="H493" s="18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="I493" s="39" t="s">
-        <v>257</v>
+        <v>148</v>
       </c>
       <c r="J493" s="61">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="K493" s="18" t="s">
         <v>49</v>
       </c>
       <c r="L493" s="18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M493" s="53" t="s">
         <v>205</v>
@@ -25465,7 +25531,7 @@
     </row>
     <row r="494" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B494" s="36" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D494" s="18" t="s">
         <v>410</v>
@@ -25477,13 +25543,13 @@
         <v>92</v>
       </c>
       <c r="I494" s="39" t="s">
-        <v>302</v>
+        <v>188</v>
       </c>
       <c r="J494" s="61">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="K494" s="18" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="L494" s="18" t="s">
         <v>39</v>
@@ -25499,7 +25565,7 @@
     </row>
     <row r="495" spans="2:22" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B495" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D495" s="18" t="s">
         <v>410</v>
@@ -25511,13 +25577,13 @@
         <v>92</v>
       </c>
       <c r="I495" s="39" t="s">
-        <v>303</v>
+        <v>188</v>
       </c>
       <c r="J495" s="61">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="K495" s="18" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="L495" s="18" t="s">
         <v>39</v>
@@ -25545,16 +25611,16 @@
         <v>92</v>
       </c>
       <c r="I496" s="39" t="s">
-        <v>303</v>
+        <v>257</v>
       </c>
       <c r="J496" s="61">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="K496" s="18" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="L496" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M496" s="53" t="s">
         <v>205</v>
@@ -25565,17 +25631,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A497" s="36"/>
+    <row r="497" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B497" s="36" t="s">
         <v>292</v>
       </c>
-      <c r="C497" s="36"/>
       <c r="D497" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="E497" s="36"/>
-      <c r="F497" s="36"/>
       <c r="G497" s="20" t="s">
         <v>291</v>
       </c>
@@ -25583,46 +25645,33 @@
         <v>92</v>
       </c>
       <c r="I497" s="39" t="s">
-        <v>303</v>
+        <v>257</v>
       </c>
       <c r="J497" s="61">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="K497" s="18" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="L497" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M497" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N497" s="37"/>
-      <c r="O497" s="36"/>
-      <c r="P497" s="36"/>
-      <c r="Q497" s="36"/>
-      <c r="R497" s="36"/>
-      <c r="S497" s="36"/>
-      <c r="T497" s="36"/>
-      <c r="U497" s="36"/>
       <c r="V497" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W497" s="36"/>
-      <c r="X497" s="36"/>
-    </row>
-    <row r="498" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A498" s="36"/>
+    </row>
+    <row r="498" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B498" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="C498" s="36"/>
       <c r="D498" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="E498" s="36"/>
-      <c r="F498" s="36"/>
       <c r="G498" s="20" t="s">
         <v>291</v>
       </c>
@@ -25630,60 +25679,47 @@
         <v>92</v>
       </c>
       <c r="I498" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J498" s="61">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="K498" s="18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="L498" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M498" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N498" s="37"/>
-      <c r="O498" s="36"/>
-      <c r="P498" s="36"/>
-      <c r="Q498" s="36"/>
-      <c r="R498" s="36"/>
-      <c r="S498" s="36"/>
-      <c r="T498" s="36"/>
-      <c r="U498" s="36"/>
       <c r="V498" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W498" s="36"/>
-      <c r="X498" s="36"/>
-    </row>
-    <row r="499" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A499" s="36"/>
+    </row>
+    <row r="499" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B499" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="C499" s="36"/>
       <c r="D499" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="E499" s="36"/>
-      <c r="F499" s="36"/>
       <c r="G499" s="20" t="s">
         <v>291</v>
       </c>
       <c r="H499" s="18" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="I499" s="39" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J499" s="61">
-        <v>405</v>
+        <v>361</v>
       </c>
       <c r="K499" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L499" s="18" t="s">
         <v>39</v>
@@ -25692,73 +25728,49 @@
         <v>205</v>
       </c>
       <c r="N499" s="37"/>
-      <c r="O499" s="36"/>
-      <c r="P499" s="36"/>
-      <c r="Q499" s="36"/>
-      <c r="R499" s="36"/>
-      <c r="S499" s="36"/>
-      <c r="T499" s="36"/>
-      <c r="U499" s="36"/>
       <c r="V499" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W499" s="36"/>
-      <c r="X499" s="36"/>
-    </row>
-    <row r="500" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A500" s="36"/>
+    </row>
+    <row r="500" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B500" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="C500" s="36"/>
+        <v>290</v>
+      </c>
       <c r="D500" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="E500" s="36"/>
-      <c r="F500" s="36"/>
       <c r="G500" s="20" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="H500" s="18" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="I500" s="39" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="J500" s="61">
-        <v>137</v>
+        <v>361</v>
       </c>
       <c r="K500" s="18" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="L500" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M500" s="53"/>
+        <v>49</v>
+      </c>
+      <c r="M500" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N500" s="37"/>
-      <c r="O500" s="36"/>
-      <c r="P500" s="36"/>
-      <c r="Q500" s="36" t="s">
-        <v>336</v>
-      </c>
-      <c r="R500" s="36" t="s">
-        <v>399</v>
-      </c>
-      <c r="S500" s="36"/>
-      <c r="T500" s="36"/>
-      <c r="U500" s="36"/>
       <c r="V500" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W500" s="36"/>
-      <c r="X500" s="36"/>
     </row>
     <row r="501" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A501" s="36"/>
       <c r="B501" s="36" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="C501" s="36"/>
       <c r="D501" s="18" t="s">
@@ -25767,22 +25779,22 @@
       <c r="E501" s="36"/>
       <c r="F501" s="36"/>
       <c r="G501" s="20" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="H501" s="18" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="I501" s="39" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J501" s="61">
-        <v>154</v>
+        <v>361</v>
       </c>
       <c r="K501" s="18" t="s">
         <v>38</v>
       </c>
       <c r="L501" s="18" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="M501" s="53" t="s">
         <v>205</v>
@@ -25791,9 +25803,7 @@
       <c r="O501" s="36"/>
       <c r="P501" s="36"/>
       <c r="Q501" s="36"/>
-      <c r="R501" s="36" t="s">
-        <v>242</v>
-      </c>
+      <c r="R501" s="36"/>
       <c r="S501" s="36"/>
       <c r="T501" s="36"/>
       <c r="U501" s="36"/>
@@ -25807,7 +25817,7 @@
     <row r="502" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A502" s="36"/>
       <c r="B502" s="36" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="C502" s="36"/>
       <c r="D502" s="18" t="s">
@@ -25816,22 +25826,22 @@
       <c r="E502" s="36"/>
       <c r="F502" s="36"/>
       <c r="G502" s="20" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="H502" s="18" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I502" s="39" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="J502" s="61">
-        <v>173</v>
+        <v>363</v>
       </c>
       <c r="K502" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L502" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M502" s="53" t="s">
         <v>205</v>
@@ -25840,9 +25850,7 @@
       <c r="O502" s="36"/>
       <c r="P502" s="36"/>
       <c r="Q502" s="36"/>
-      <c r="R502" s="36" t="s">
-        <v>242</v>
-      </c>
+      <c r="R502" s="36"/>
       <c r="S502" s="36"/>
       <c r="T502" s="36"/>
       <c r="U502" s="36"/>
@@ -25856,7 +25864,7 @@
     <row r="503" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A503" s="36"/>
       <c r="B503" s="36" t="s">
-        <v>508</v>
+        <v>294</v>
       </c>
       <c r="C503" s="36"/>
       <c r="D503" s="18" t="s">
@@ -25865,19 +25873,19 @@
       <c r="E503" s="36"/>
       <c r="F503" s="36"/>
       <c r="G503" s="20" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="H503" s="18" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="I503" s="39" t="s">
-        <v>309</v>
-      </c>
-      <c r="J503" s="61" t="s">
-        <v>477</v>
+        <v>305</v>
+      </c>
+      <c r="J503" s="61">
+        <v>405</v>
       </c>
       <c r="K503" s="18" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="L503" s="18" t="s">
         <v>39</v>
@@ -25889,9 +25897,7 @@
       <c r="O503" s="36"/>
       <c r="P503" s="36"/>
       <c r="Q503" s="36"/>
-      <c r="R503" s="36" t="s">
-        <v>242</v>
-      </c>
+      <c r="R503" s="36"/>
       <c r="S503" s="36"/>
       <c r="T503" s="36"/>
       <c r="U503" s="36"/>
@@ -25917,29 +25923,29 @@
         <v>307</v>
       </c>
       <c r="H504" s="18" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="I504" s="39" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="J504" s="61">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="K504" s="18" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="L504" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="M504" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="M504" s="53"/>
       <c r="N504" s="37"/>
       <c r="O504" s="36"/>
       <c r="P504" s="36"/>
-      <c r="Q504" s="36"/>
+      <c r="Q504" s="36" t="s">
+        <v>336</v>
+      </c>
       <c r="R504" s="36" t="s">
-        <v>242</v>
+        <v>399</v>
       </c>
       <c r="S504" s="36"/>
       <c r="T504" s="36"/>
@@ -25966,16 +25972,16 @@
         <v>307</v>
       </c>
       <c r="H505" s="18" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="I505" s="39" t="s">
-        <v>100</v>
+        <v>308</v>
       </c>
       <c r="J505" s="61">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="K505" s="18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="L505" s="18" t="s">
         <v>39</v>
@@ -26018,16 +26024,16 @@
         <v>99</v>
       </c>
       <c r="I506" s="39" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="J506" s="61">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="K506" s="18" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="L506" s="18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M506" s="53" t="s">
         <v>205</v>
@@ -26052,7 +26058,7 @@
     <row r="507" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A507" s="36"/>
       <c r="B507" s="36" t="s">
-        <v>306</v>
+        <v>508</v>
       </c>
       <c r="C507" s="36"/>
       <c r="D507" s="18" t="s">
@@ -26064,17 +26070,19 @@
         <v>307</v>
       </c>
       <c r="H507" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="I507" s="39"/>
-      <c r="J507" s="61">
-        <v>207</v>
+        <v>99</v>
+      </c>
+      <c r="I507" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="J507" s="61" t="s">
+        <v>477</v>
       </c>
       <c r="K507" s="18" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="L507" s="18" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="M507" s="53" t="s">
         <v>205</v>
@@ -26111,19 +26119,19 @@
         <v>307</v>
       </c>
       <c r="H508" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I508" s="39" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="J508" s="61">
-        <v>223</v>
+        <v>182</v>
       </c>
       <c r="K508" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L508" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M508" s="53" t="s">
         <v>205</v>
@@ -26145,136 +26153,176 @@
       <c r="W508" s="36"/>
       <c r="X508" s="36"/>
     </row>
-    <row r="509" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A509" s="36"/>
       <c r="B509" s="36" t="s">
-        <v>401</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C509" s="36"/>
       <c r="D509" s="18" t="s">
         <v>410</v>
       </c>
+      <c r="E509" s="36"/>
+      <c r="F509" s="36"/>
       <c r="G509" s="20" t="s">
         <v>307</v>
       </c>
       <c r="H509" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I509" s="39"/>
+        <v>99</v>
+      </c>
+      <c r="I509" s="39" t="s">
+        <v>100</v>
+      </c>
       <c r="J509" s="61">
-        <v>257</v>
+        <v>190</v>
       </c>
       <c r="K509" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L509" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M509" s="53"/>
+        <v>39</v>
+      </c>
+      <c r="M509" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N509" s="37"/>
-      <c r="Q509" s="36" t="s">
-        <v>329</v>
-      </c>
+      <c r="O509" s="36"/>
+      <c r="P509" s="36"/>
+      <c r="Q509" s="36"/>
       <c r="R509" s="36" t="s">
-        <v>400</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="S509" s="36"/>
+      <c r="T509" s="36"/>
+      <c r="U509" s="36"/>
       <c r="V509" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="510" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W509" s="36"/>
+      <c r="X509" s="36"/>
+    </row>
+    <row r="510" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A510" s="36"/>
       <c r="B510" s="36" t="s">
-        <v>401</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C510" s="36"/>
       <c r="D510" s="18" t="s">
         <v>410</v>
       </c>
+      <c r="E510" s="36"/>
+      <c r="F510" s="36"/>
       <c r="G510" s="20" t="s">
         <v>307</v>
       </c>
       <c r="H510" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I510" s="39"/>
+        <v>99</v>
+      </c>
+      <c r="I510" s="39" t="s">
+        <v>293</v>
+      </c>
       <c r="J510" s="61">
-        <v>258</v>
+        <v>193</v>
       </c>
       <c r="K510" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L510" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="M510" s="53"/>
+        <v>44</v>
+      </c>
+      <c r="M510" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N510" s="37"/>
-      <c r="Q510" s="36" t="s">
-        <v>329</v>
-      </c>
+      <c r="O510" s="36"/>
+      <c r="P510" s="36"/>
+      <c r="Q510" s="36"/>
       <c r="R510" s="36" t="s">
-        <v>400</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="S510" s="36"/>
+      <c r="T510" s="36"/>
+      <c r="U510" s="36"/>
       <c r="V510" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="511" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W510" s="36"/>
+      <c r="X510" s="36"/>
+    </row>
+    <row r="511" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A511" s="36"/>
       <c r="B511" s="36" t="s">
         <v>306</v>
       </c>
+      <c r="C511" s="36"/>
       <c r="D511" s="18" t="s">
         <v>410</v>
       </c>
+      <c r="E511" s="36"/>
+      <c r="F511" s="36"/>
       <c r="G511" s="20" t="s">
         <v>307</v>
       </c>
       <c r="H511" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I511" s="39" t="s">
-        <v>311</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I511" s="39"/>
       <c r="J511" s="61">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="K511" s="18" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="L511" s="18" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="M511" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N511" s="37"/>
+      <c r="O511" s="36"/>
+      <c r="P511" s="36"/>
+      <c r="Q511" s="36"/>
       <c r="R511" s="36" t="s">
         <v>242</v>
       </c>
+      <c r="S511" s="36"/>
+      <c r="T511" s="36"/>
+      <c r="U511" s="36"/>
       <c r="V511" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="512" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W511" s="36"/>
+      <c r="X511" s="36"/>
+    </row>
+    <row r="512" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A512" s="36"/>
       <c r="B512" s="36" t="s">
         <v>306</v>
       </c>
+      <c r="C512" s="36"/>
       <c r="D512" s="18" t="s">
         <v>410</v>
       </c>
+      <c r="E512" s="36"/>
+      <c r="F512" s="36"/>
       <c r="G512" s="20" t="s">
         <v>307</v>
       </c>
       <c r="H512" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I512" s="39" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
       <c r="J512" s="61">
-        <v>344</v>
+        <v>223</v>
       </c>
       <c r="K512" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="L512" s="18" t="s">
         <v>39</v>
@@ -26283,17 +26331,25 @@
         <v>205</v>
       </c>
       <c r="N512" s="37"/>
+      <c r="O512" s="36"/>
+      <c r="P512" s="36"/>
+      <c r="Q512" s="36"/>
       <c r="R512" s="36" t="s">
         <v>242</v>
       </c>
+      <c r="S512" s="36"/>
+      <c r="T512" s="36"/>
+      <c r="U512" s="36"/>
       <c r="V512" s="36" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="W512" s="36"/>
+      <c r="X512" s="36"/>
     </row>
     <row r="513" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B513" s="36" t="s">
-        <v>306</v>
+        <v>401</v>
       </c>
       <c r="D513" s="18" t="s">
         <v>410</v>
@@ -26302,26 +26358,25 @@
         <v>307</v>
       </c>
       <c r="H513" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I513" s="39" t="s">
-        <v>245</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="I513" s="39"/>
       <c r="J513" s="61">
-        <v>362</v>
+        <v>257</v>
       </c>
       <c r="K513" s="18" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="L513" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="M513" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M513" s="53"/>
       <c r="N513" s="37"/>
+      <c r="Q513" s="36" t="s">
+        <v>329</v>
+      </c>
       <c r="R513" s="36" t="s">
-        <v>242</v>
+        <v>400</v>
       </c>
       <c r="V513" s="36" t="b">
         <f t="shared" si="7"/>
@@ -26330,7 +26385,7 @@
     </row>
     <row r="514" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B514" s="36" t="s">
-        <v>306</v>
+        <v>401</v>
       </c>
       <c r="D514" s="18" t="s">
         <v>410</v>
@@ -26339,268 +26394,252 @@
         <v>307</v>
       </c>
       <c r="H514" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="I514" s="39" t="s">
-        <v>271</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="I514" s="39"/>
       <c r="J514" s="61">
-        <v>387</v>
+        <v>258</v>
       </c>
       <c r="K514" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L514" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M514" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="M514" s="53"/>
       <c r="N514" s="37"/>
+      <c r="Q514" s="36" t="s">
+        <v>329</v>
+      </c>
       <c r="R514" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="V514" s="36" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="515" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B515" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="D515" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="G515" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="H515" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I515" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="J515" s="61">
+        <v>276</v>
+      </c>
+      <c r="K515" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L515" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M515" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="N515" s="37"/>
+      <c r="R515" s="36" t="s">
         <v>242</v>
       </c>
-      <c r="V514" s="36" t="b">
-        <f t="shared" ref="V514:V541" si="8">AND(ISBLANK(M514),ISBLANK(N514),ISBLANK(O514),ISBLANK(P514),ISBLANK(Q514))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="515" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D515" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G515" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="H515" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="I515" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="J515" s="61">
-        <v>579</v>
-      </c>
-      <c r="K515" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="L515" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M515" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N515" s="37"/>
       <c r="V515" s="36" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="516" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B516" s="36" t="s">
-        <v>516</v>
+        <v>306</v>
       </c>
       <c r="D516" s="18" t="s">
-        <v>49</v>
+        <v>410</v>
       </c>
       <c r="G516" s="20" t="s">
-        <v>158</v>
+        <v>307</v>
       </c>
       <c r="H516" s="18" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I516" s="39" t="s">
-        <v>293</v>
-      </c>
-      <c r="J516" s="61" t="s">
-        <v>517</v>
+        <v>188</v>
+      </c>
+      <c r="J516" s="61">
+        <v>344</v>
       </c>
       <c r="K516" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L516" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="M516" s="53"/>
+        <v>39</v>
+      </c>
+      <c r="M516" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N516" s="37"/>
-      <c r="Q516" s="36" t="s">
-        <v>336</v>
-      </c>
       <c r="R516" s="36" t="s">
-        <v>384</v>
+        <v>242</v>
       </c>
       <c r="V516" s="36" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="517" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B517" s="36" t="s">
-        <v>518</v>
+        <v>306</v>
       </c>
       <c r="D517" s="18" t="s">
-        <v>49</v>
+        <v>410</v>
       </c>
       <c r="G517" s="20" t="s">
-        <v>158</v>
+        <v>307</v>
       </c>
       <c r="H517" s="18" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I517" s="39" t="s">
-        <v>293</v>
-      </c>
-      <c r="J517" s="61" t="s">
-        <v>517</v>
+        <v>245</v>
+      </c>
+      <c r="J517" s="61">
+        <v>362</v>
       </c>
       <c r="K517" s="18" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="L517" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="M517" s="53"/>
+        <v>44</v>
+      </c>
+      <c r="M517" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N517" s="37"/>
-      <c r="Q517" s="36" t="s">
-        <v>336</v>
-      </c>
       <c r="R517" s="36" t="s">
-        <v>384</v>
+        <v>242</v>
       </c>
       <c r="V517" s="36" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="518" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B518" s="36" t="s">
-        <v>376</v>
+        <v>306</v>
       </c>
       <c r="D518" s="18" t="s">
-        <v>49</v>
+        <v>410</v>
       </c>
       <c r="G518" s="20" t="s">
-        <v>158</v>
+        <v>307</v>
       </c>
       <c r="H518" s="18" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="I518" s="39" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="J518" s="61">
-        <v>634</v>
+        <v>387</v>
       </c>
       <c r="K518" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L518" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="M518" s="53"/>
+        <v>39</v>
+      </c>
+      <c r="M518" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N518" s="37"/>
-      <c r="Q518" s="36" t="s">
-        <v>336</v>
-      </c>
       <c r="R518" s="36" t="s">
-        <v>384</v>
+        <v>242</v>
       </c>
       <c r="V518" s="36" t="b">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="519" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A519" s="36"/>
-      <c r="B519" s="36"/>
-      <c r="C519" s="36"/>
+        <f t="shared" ref="V518:V541" si="8">AND(ISBLANK(M518),ISBLANK(N518),ISBLANK(O518),ISBLANK(P518),ISBLANK(Q518))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D519" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E519" s="36"/>
-      <c r="F519" s="36"/>
       <c r="G519" s="20" t="s">
         <v>158</v>
       </c>
       <c r="H519" s="18" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="I519" s="39" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="J519" s="61">
-        <v>667</v>
+        <v>579</v>
       </c>
       <c r="K519" s="18" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="L519" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M519" s="53" t="s">
         <v>205</v>
       </c>
       <c r="N519" s="37"/>
-      <c r="O519" s="36"/>
-      <c r="P519" s="36"/>
-      <c r="Q519" s="36"/>
-      <c r="R519" s="36"/>
-      <c r="S519" s="36"/>
-      <c r="T519" s="36"/>
-      <c r="U519" s="36"/>
       <c r="V519" s="36" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="W519" s="36"/>
-      <c r="X519" s="36"/>
-    </row>
-    <row r="520" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A520" s="36"/>
-      <c r="B520" s="36"/>
-      <c r="C520" s="36"/>
+    </row>
+    <row r="520" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B520" s="36" t="s">
+        <v>516</v>
+      </c>
       <c r="D520" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E520" s="36"/>
-      <c r="F520" s="36"/>
       <c r="G520" s="20" t="s">
         <v>158</v>
       </c>
       <c r="H520" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I520" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="J520" s="61">
-        <v>669</v>
+        <v>293</v>
+      </c>
+      <c r="J520" s="61" t="s">
+        <v>517</v>
       </c>
       <c r="K520" s="18" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="L520" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M520" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N520" s="64"/>
-      <c r="O520" s="36"/>
-      <c r="P520" s="36"/>
-      <c r="Q520" s="36"/>
-      <c r="R520" s="36"/>
-      <c r="S520" s="36"/>
-      <c r="T520" s="36"/>
-      <c r="U520" s="36"/>
+        <v>249</v>
+      </c>
+      <c r="M520" s="53"/>
+      <c r="N520" s="37"/>
+      <c r="Q520" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="R520" s="36" t="s">
+        <v>384</v>
+      </c>
       <c r="V520" s="36" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="W520" s="36"/>
-      <c r="X520" s="36"/>
     </row>
     <row r="521" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B521" s="36" t="s">
+        <v>518</v>
+      </c>
       <c r="D521" s="18" t="s">
         <v>49</v>
       </c>
@@ -26608,22 +26647,28 @@
         <v>158</v>
       </c>
       <c r="H521" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I521" s="39"/>
-      <c r="J521" s="61">
-        <v>675</v>
+        <v>99</v>
+      </c>
+      <c r="I521" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="J521" s="61" t="s">
+        <v>517</v>
       </c>
       <c r="K521" s="18" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="L521" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M521" s="53" t="s">
-        <v>205</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="M521" s="53"/>
       <c r="N521" s="37"/>
+      <c r="Q521" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="R521" s="36" t="s">
+        <v>384</v>
+      </c>
       <c r="V521" s="36" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -26640,13 +26685,13 @@
         <v>158</v>
       </c>
       <c r="H522" s="18" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="I522" s="39" t="s">
-        <v>377</v>
+        <v>293</v>
       </c>
       <c r="J522" s="61">
-        <v>691</v>
+        <v>634</v>
       </c>
       <c r="K522" s="18" t="s">
         <v>49</v>
@@ -26680,24 +26725,24 @@
         <v>158</v>
       </c>
       <c r="H523" s="18" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I523" s="39" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="J523" s="61">
-        <v>742</v>
+        <v>667</v>
       </c>
       <c r="K523" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L523" s="18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="M523" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="N523" s="64"/>
+      <c r="N523" s="37"/>
       <c r="O523" s="36"/>
       <c r="P523" s="36"/>
       <c r="Q523" s="36"/>
@@ -26725,16 +26770,16 @@
         <v>158</v>
       </c>
       <c r="H524" s="18" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I524" s="39" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="J524" s="61">
-        <v>753</v>
+        <v>669</v>
       </c>
       <c r="K524" s="18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L524" s="18" t="s">
         <v>39</v>
@@ -26742,7 +26787,7 @@
       <c r="M524" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="N524" s="37"/>
+      <c r="N524" s="64"/>
       <c r="O524" s="36"/>
       <c r="P524" s="36"/>
       <c r="Q524" s="36"/>
@@ -26757,239 +26802,256 @@
       <c r="W524" s="36"/>
       <c r="X524" s="36"/>
     </row>
-    <row r="525" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A525" s="36"/>
-      <c r="B525" s="36" t="s">
-        <v>529</v>
-      </c>
-      <c r="C525" s="36"/>
+    <row r="525" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D525" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E525" s="36"/>
-      <c r="F525" s="36"/>
+        <v>49</v>
+      </c>
       <c r="G525" s="20" t="s">
-        <v>530</v>
+        <v>158</v>
       </c>
       <c r="H525" s="18" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I525" s="39"/>
       <c r="J525" s="61">
-        <v>163</v>
+        <v>675</v>
       </c>
       <c r="K525" s="18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="L525" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M525" s="53"/>
+        <v>1</v>
+      </c>
+      <c r="M525" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="N525" s="37"/>
-      <c r="O525" s="36"/>
-      <c r="P525" s="36"/>
-      <c r="Q525" s="36" t="s">
-        <v>554</v>
-      </c>
-      <c r="R525" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="S525" s="36"/>
-      <c r="T525" s="36"/>
-      <c r="U525" s="36"/>
       <c r="V525" s="36" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="W525" s="36"/>
-      <c r="X525" s="36"/>
-    </row>
-    <row r="526" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A526" s="36"/>
+    </row>
+    <row r="526" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B526" s="36" t="s">
-        <v>535</v>
-      </c>
-      <c r="C526" s="36"/>
+        <v>376</v>
+      </c>
       <c r="D526" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E526" s="36"/>
-      <c r="F526" s="36"/>
-      <c r="G526" s="130" t="s">
-        <v>530</v>
-      </c>
-      <c r="H526" s="131" t="s">
-        <v>105</v>
-      </c>
-      <c r="I526" s="132"/>
+        <v>49</v>
+      </c>
+      <c r="G526" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H526" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I526" s="39" t="s">
+        <v>377</v>
+      </c>
       <c r="J526" s="61">
-        <v>163</v>
+        <v>691</v>
       </c>
       <c r="K526" s="18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L526" s="18" t="s">
-        <v>39</v>
+        <v>249</v>
       </c>
       <c r="M526" s="53"/>
       <c r="N526" s="37"/>
-      <c r="O526" s="36"/>
-      <c r="P526" s="36"/>
       <c r="Q526" s="36" t="s">
-        <v>554</v>
+        <v>336</v>
       </c>
       <c r="R526" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="S526" s="36"/>
-      <c r="T526" s="36"/>
-      <c r="U526" s="36"/>
+        <v>384</v>
+      </c>
       <c r="V526" s="36" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="W526" s="36"/>
-      <c r="X526" s="36"/>
     </row>
     <row r="527" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B527" s="71" t="s">
+      <c r="A527" s="36"/>
+      <c r="B527" s="36"/>
+      <c r="C527" s="36"/>
+      <c r="D527" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E527" s="36"/>
+      <c r="F527" s="36"/>
+      <c r="G527" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H527" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I527" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="J527" s="61">
+        <v>742</v>
+      </c>
+      <c r="K527" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L527" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M527" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="N527" s="64"/>
+      <c r="O527" s="36"/>
+      <c r="P527" s="36"/>
+      <c r="Q527" s="36"/>
+      <c r="R527" s="36"/>
+      <c r="S527" s="36"/>
+      <c r="T527" s="36"/>
+      <c r="U527" s="36"/>
+      <c r="V527" s="36" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W527" s="36"/>
+      <c r="X527" s="36"/>
+    </row>
+    <row r="528" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A528" s="36"/>
+      <c r="B528" s="36"/>
+      <c r="C528" s="36"/>
+      <c r="D528" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E528" s="36"/>
+      <c r="F528" s="36"/>
+      <c r="G528" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H528" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I528" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="J528" s="61">
+        <v>753</v>
+      </c>
+      <c r="K528" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L528" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M528" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="N528" s="37"/>
+      <c r="O528" s="36"/>
+      <c r="P528" s="36"/>
+      <c r="Q528" s="36"/>
+      <c r="R528" s="36"/>
+      <c r="S528" s="36"/>
+      <c r="T528" s="36"/>
+      <c r="U528" s="36"/>
+      <c r="V528" s="36" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W528" s="36"/>
+      <c r="X528" s="36"/>
+    </row>
+    <row r="529" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A529" s="36"/>
+      <c r="B529" s="36" t="s">
         <v>529</v>
       </c>
-      <c r="D527" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G527" s="73" t="s">
-        <v>530</v>
-      </c>
-      <c r="H527" s="72" t="s">
-        <v>122</v>
-      </c>
-      <c r="I527" s="74" t="s">
-        <v>163</v>
-      </c>
-      <c r="J527" s="103">
-        <v>227</v>
-      </c>
-      <c r="K527" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="L527" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="M527" s="76"/>
-      <c r="N527" s="77"/>
-      <c r="R527" s="71" t="s">
-        <v>226</v>
-      </c>
-      <c r="V527" s="71" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="528" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B528" s="71" t="s">
-        <v>535</v>
-      </c>
-      <c r="D528" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G528" s="73" t="s">
-        <v>530</v>
-      </c>
-      <c r="H528" s="72" t="s">
-        <v>122</v>
-      </c>
-      <c r="I528" s="74" t="s">
-        <v>163</v>
-      </c>
-      <c r="J528" s="103">
-        <v>227</v>
-      </c>
-      <c r="K528" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="L528" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="M528" s="76"/>
-      <c r="N528" s="77"/>
-      <c r="R528" s="71" t="s">
-        <v>226</v>
-      </c>
-      <c r="V528" s="71" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="529" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B529" s="71" t="s">
-        <v>529</v>
-      </c>
+      <c r="C529" s="36"/>
       <c r="D529" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G529" s="73" t="s">
+      <c r="E529" s="36"/>
+      <c r="F529" s="36"/>
+      <c r="G529" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="H529" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="I529" s="74" t="s">
-        <v>531</v>
-      </c>
-      <c r="J529" s="103">
-        <v>249</v>
-      </c>
-      <c r="K529" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="L529" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="M529" s="76"/>
-      <c r="N529" s="77"/>
-      <c r="R529" s="71" t="s">
+      <c r="H529" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I529" s="39"/>
+      <c r="J529" s="61">
+        <v>163</v>
+      </c>
+      <c r="K529" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L529" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M529" s="53"/>
+      <c r="N529" s="37"/>
+      <c r="O529" s="36"/>
+      <c r="P529" s="36"/>
+      <c r="Q529" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="R529" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="V529" s="71" t="b">
+      <c r="S529" s="36"/>
+      <c r="T529" s="36"/>
+      <c r="U529" s="36"/>
+      <c r="V529" s="36" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W529" s="36"/>
+      <c r="X529" s="36"/>
     </row>
     <row r="530" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B530" s="71" t="s">
+      <c r="A530" s="36"/>
+      <c r="B530" s="36" t="s">
         <v>535</v>
       </c>
+      <c r="C530" s="36"/>
       <c r="D530" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G530" s="73" t="s">
+      <c r="E530" s="36"/>
+      <c r="F530" s="36"/>
+      <c r="G530" s="130" t="s">
         <v>530</v>
       </c>
-      <c r="H530" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="I530" s="74" t="s">
-        <v>531</v>
-      </c>
-      <c r="J530" s="103">
-        <v>249</v>
-      </c>
-      <c r="K530" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="L530" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="M530" s="76"/>
-      <c r="N530" s="77"/>
-      <c r="R530" s="71" t="s">
+      <c r="H530" s="131" t="s">
+        <v>105</v>
+      </c>
+      <c r="I530" s="132"/>
+      <c r="J530" s="61">
+        <v>163</v>
+      </c>
+      <c r="K530" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L530" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M530" s="53"/>
+      <c r="N530" s="37"/>
+      <c r="O530" s="36"/>
+      <c r="P530" s="36"/>
+      <c r="Q530" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="R530" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="V530" s="71" t="b">
+      <c r="S530" s="36"/>
+      <c r="T530" s="36"/>
+      <c r="U530" s="36"/>
+      <c r="V530" s="36" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W530" s="36"/>
+      <c r="X530" s="36"/>
     </row>
     <row r="531" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B531" s="71" t="s">
@@ -26998,21 +27060,23 @@
       <c r="D531" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G531" s="135" t="s">
+      <c r="G531" s="73" t="s">
         <v>530</v>
       </c>
-      <c r="H531" s="136" t="s">
-        <v>124</v>
-      </c>
-      <c r="I531" s="137"/>
+      <c r="H531" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="I531" s="74" t="s">
+        <v>163</v>
+      </c>
       <c r="J531" s="103">
-        <v>282</v>
+        <v>227</v>
       </c>
       <c r="K531" s="72" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="L531" s="72" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="M531" s="76"/>
       <c r="N531" s="77"/>
@@ -27035,17 +27099,19 @@
         <v>530</v>
       </c>
       <c r="H532" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="I532" s="74"/>
+        <v>122</v>
+      </c>
+      <c r="I532" s="74" t="s">
+        <v>163</v>
+      </c>
       <c r="J532" s="103">
-        <v>282</v>
+        <v>227</v>
       </c>
       <c r="K532" s="72" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="L532" s="72" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="M532" s="76"/>
       <c r="N532" s="77"/>
@@ -27064,20 +27130,20 @@
       <c r="D533" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G533" s="135" t="s">
+      <c r="G533" s="73" t="s">
         <v>530</v>
       </c>
-      <c r="H533" s="136" t="s">
-        <v>92</v>
-      </c>
-      <c r="I533" s="137" t="s">
-        <v>532</v>
+      <c r="H533" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="I533" s="74" t="s">
+        <v>531</v>
       </c>
       <c r="J533" s="103">
-        <v>468</v>
+        <v>249</v>
       </c>
       <c r="K533" s="72" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L533" s="72" t="s">
         <v>39</v>
@@ -27099,22 +27165,22 @@
       <c r="D534" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G534" s="135" t="s">
+      <c r="G534" s="73" t="s">
         <v>530</v>
       </c>
-      <c r="H534" s="136" t="s">
-        <v>92</v>
-      </c>
-      <c r="I534" s="137" t="s">
-        <v>532</v>
-      </c>
-      <c r="J534" s="138">
-        <v>468</v>
-      </c>
-      <c r="K534" s="136" t="s">
-        <v>48</v>
-      </c>
-      <c r="L534" s="136" t="s">
+      <c r="H534" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="I534" s="74" t="s">
+        <v>531</v>
+      </c>
+      <c r="J534" s="103">
+        <v>249</v>
+      </c>
+      <c r="K534" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="L534" s="72" t="s">
         <v>39</v>
       </c>
       <c r="M534" s="76"/>
@@ -27128,206 +27194,140 @@
       </c>
     </row>
     <row r="535" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A535" s="36"/>
-      <c r="B535" s="36" t="s">
-        <v>482</v>
-      </c>
-      <c r="C535" s="36"/>
+      <c r="B535" s="71" t="s">
+        <v>529</v>
+      </c>
       <c r="D535" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E535" s="36"/>
-      <c r="F535" s="36"/>
-      <c r="G535" s="20" t="s">
-        <v>483</v>
-      </c>
-      <c r="H535" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="I535" s="39" t="s">
-        <v>484</v>
-      </c>
-      <c r="J535" s="139">
-        <v>83</v>
-      </c>
-      <c r="K535" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="L535" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M535" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N535" s="37"/>
-      <c r="O535" s="36"/>
-      <c r="P535" s="36"/>
-      <c r="Q535" s="36"/>
-      <c r="R535" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="S535" s="36"/>
-      <c r="T535" s="36"/>
-      <c r="U535" s="36"/>
-      <c r="V535" s="36" t="b">
+      <c r="G535" s="135" t="s">
+        <v>530</v>
+      </c>
+      <c r="H535" s="136" t="s">
+        <v>124</v>
+      </c>
+      <c r="I535" s="137"/>
+      <c r="J535" s="103">
+        <v>282</v>
+      </c>
+      <c r="K535" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="L535" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="M535" s="76"/>
+      <c r="N535" s="77"/>
+      <c r="R535" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="V535" s="71" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="W535" s="36" t="s">
-        <v>523</v>
-      </c>
-      <c r="X535" s="36"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="536" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A536" s="36"/>
-      <c r="B536" s="36" t="s">
-        <v>482</v>
-      </c>
-      <c r="C536" s="36"/>
+      <c r="B536" s="71" t="s">
+        <v>535</v>
+      </c>
       <c r="D536" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E536" s="36"/>
-      <c r="F536" s="36"/>
-      <c r="G536" s="20" t="s">
-        <v>483</v>
-      </c>
-      <c r="H536" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I536" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="J536" s="139">
-        <v>88</v>
-      </c>
-      <c r="K536" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="L536" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M536" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N536" s="37"/>
-      <c r="O536" s="36"/>
-      <c r="P536" s="36"/>
-      <c r="Q536" s="36"/>
-      <c r="R536" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="S536" s="36"/>
-      <c r="T536" s="36"/>
-      <c r="U536" s="36"/>
-      <c r="V536" s="36" t="b">
+      <c r="G536" s="73" t="s">
+        <v>530</v>
+      </c>
+      <c r="H536" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="I536" s="74"/>
+      <c r="J536" s="103">
+        <v>282</v>
+      </c>
+      <c r="K536" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="L536" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="M536" s="76"/>
+      <c r="N536" s="77"/>
+      <c r="R536" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="V536" s="71" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="W536" s="36" t="s">
-        <v>523</v>
-      </c>
-      <c r="X536" s="36"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="537" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A537" s="36"/>
-      <c r="B537" s="36" t="s">
-        <v>482</v>
-      </c>
-      <c r="C537" s="36"/>
+      <c r="B537" s="71" t="s">
+        <v>529</v>
+      </c>
       <c r="D537" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E537" s="36"/>
-      <c r="F537" s="36"/>
-      <c r="G537" s="20" t="s">
-        <v>483</v>
-      </c>
-      <c r="H537" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="I537" s="39" t="s">
-        <v>253</v>
-      </c>
-      <c r="J537" s="139">
-        <v>212</v>
-      </c>
-      <c r="K537" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L537" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M537" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N537" s="37"/>
-      <c r="O537" s="36"/>
-      <c r="P537" s="36"/>
-      <c r="Q537" s="36"/>
-      <c r="R537" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="S537" s="36"/>
-      <c r="T537" s="36"/>
-      <c r="U537" s="36"/>
-      <c r="V537" s="36" t="b">
+      <c r="G537" s="135" t="s">
+        <v>530</v>
+      </c>
+      <c r="H537" s="136" t="s">
+        <v>92</v>
+      </c>
+      <c r="I537" s="137" t="s">
+        <v>532</v>
+      </c>
+      <c r="J537" s="103">
+        <v>468</v>
+      </c>
+      <c r="K537" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="L537" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="M537" s="76"/>
+      <c r="N537" s="77"/>
+      <c r="R537" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="V537" s="71" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="W537" s="36" t="s">
-        <v>523</v>
-      </c>
-      <c r="X537" s="36"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="538" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A538" s="36"/>
-      <c r="B538" s="36" t="s">
-        <v>482</v>
-      </c>
-      <c r="C538" s="36"/>
+      <c r="B538" s="71" t="s">
+        <v>535</v>
+      </c>
       <c r="D538" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E538" s="36"/>
-      <c r="F538" s="36"/>
-      <c r="G538" s="20" t="s">
-        <v>483</v>
-      </c>
-      <c r="H538" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="I538" s="39"/>
-      <c r="J538" s="139">
-        <v>309</v>
-      </c>
-      <c r="K538" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="L538" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="M538" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="N538" s="37"/>
-      <c r="O538" s="36"/>
-      <c r="P538" s="36"/>
-      <c r="Q538" s="36"/>
-      <c r="R538" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="S538" s="36"/>
-      <c r="T538" s="36"/>
-      <c r="U538" s="36"/>
-      <c r="V538" s="36" t="b">
+      <c r="G538" s="135" t="s">
+        <v>530</v>
+      </c>
+      <c r="H538" s="136" t="s">
+        <v>92</v>
+      </c>
+      <c r="I538" s="137" t="s">
+        <v>532</v>
+      </c>
+      <c r="J538" s="138">
+        <v>468</v>
+      </c>
+      <c r="K538" s="136" t="s">
+        <v>48</v>
+      </c>
+      <c r="L538" s="136" t="s">
+        <v>39</v>
+      </c>
+      <c r="M538" s="76"/>
+      <c r="N538" s="77"/>
+      <c r="R538" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="V538" s="71" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="W538" s="36" t="s">
-        <v>523</v>
-      </c>
-      <c r="X538" s="36"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="539" spans="1:24" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B539" s="36" t="s">
@@ -28412,17 +28412,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="976" yWindow="308" count="7">
-    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Remark" prompt="Optional field to save any remark about the annotated data." sqref="R1 R6:R151 R155:R450 R453:R1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Remark" prompt="Optional field to save any remark about the annotated data." sqref="R1 R6:R151 R155:R454 R457:R538 R539:R1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Site / Bond / SNP" prompt="A Site / Bond / SNP that has been inserted or removed by mutation._x000a_Optional field, typically only used when the mutant AA is not A or L." sqref="O1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reference" prompt="Provide the a DOI or alternatively a PubMed ID for the original publication. If unpublished leave the cell blank (name of PI will be inserted at upload to GPCRDB)" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="PDB ID" prompt="Provide the four-letter identifier of the Xtal structure from the PDB." sqref="B44:B47 B2:B11 B15 B17:B20 B35:B36 B55 B114:B144 B164:B165 B169:B170 B250:B1048576 B86 B90:B112 B38:B41 B22:B32 B57:B84 B247:B248 B175:B245" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="UniProt identifier" prompt="Type the UniProt entry name (e.g. GRM5_HUMAN) or code (e.g. P41594) of the GPCR" sqref="G1:I1048576" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" error="You need to report a whole number" promptTitle="Sequence number" prompt="Type the sequence number (UniProt) of the mutated residue" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="PDB ID" prompt="Provide the four-letter identifier of the Xtal structure from the PDB." sqref="B44:B47 B2:B11 B15 B17:B20 B35:B36 B55 B114:B144 B164:B165 B169:B170 B86 B90:B112 B38:B41 B22:B32 B57:B84 B247:B248 B175:B245 B539:B1048576 B250:B538" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reference" prompt="Provide the a DOI or alternatively a PubMed ID for the original publication. If unpublished leave the cell blank (name of PI will be inserted at upload to GPCRDB)" sqref="A539:A1048576 A2:A538" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="UniProt identifier" prompt="Type the UniProt entry name (e.g. GRM5_HUMAN) or code (e.g. P41594) of the GPCR" sqref="G539:I1048576 G1:I538" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" error="You need to report a whole number" promptTitle="Sequence number" prompt="Type the sequence number (UniProt) of the mutated residue" sqref="J539:J1048576 J1:J538" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GCPR class" prompt="Please specify the class that the GPCR belongs to." sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GCPR class" prompt="Please specify the class that the GPCR belongs to." sqref="D539:D1048576 D2:D538" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="UniProt entry" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -28436,19 +28436,19 @@
           <x14:formula1>
             <xm:f>Droplist_Terms!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>N179 M1:M1048576</xm:sqref>
+          <xm:sqref>N179 M539:M1048576 M1:M538</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Receptor Expression" prompt="DECREASED: &gt;=20 less than Wt; UNCHANGED: 81-119% of Wt; INCREASED: &gt;=20% higher than Wt" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>Droplist_Terms!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>N180:N1048576 N103:N178 N1:N101</xm:sqref>
+          <xm:sqref>N103:N178 N1:N101 N539:N1048576 N180:N538</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Only values from the list can be used" promptTitle="Amino acid type" prompt="Select the wild-type amino acid from the list" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>Droplist_Terms!$B$2:$B$41</xm:f>
           </x14:formula1>
-          <xm:sqref>K103:K1048576 K1:K101</xm:sqref>
+          <xm:sqref>K1:K101 K539:K1048576 K103:K538</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Only values from the list can be used" promptTitle="Amino acid type" prompt="Select the mutant amino acid from the list" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -28460,37 +28460,37 @@
           <x14:formula1>
             <xm:f>Droplist_Terms!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P1:P101 P103:P1048576</xm:sqref>
+          <xm:sqref>P1:P101 P539:P1048576 P103:P538</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+          <x14:formula1>
+            <xm:f>Droplist_Terms!$I$2:$I$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>R455:R456 Q1:Q524 Q527:Q538 Q539:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Site / Bond / SNP" prompt="A Site / Bond / SNP that has been inserted or removed by mutation._x000a_Optional field, typically only used when the mutant AA is not A or L." xr:uid="{00000000-0002-0000-0000-00000C000000}">
+          <x14:formula1>
+            <xm:f>Droplist_Terms!$G$2:$G$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O101 O539:O1048576 O103:O538</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6FB0F3CC-5DA9-3745-AAA9-5F913945D9DC}">
+          <x14:formula1>
+            <xm:f>Droplist_Terms!$I$2:$I$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q525:Q526</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Ligand type" prompt="Select the type of ligand in the Xta structure from the list acoording to its effect on the receptor." xr:uid="{00000000-0002-0000-0000-00000D000000}">
           <x14:formula1>
             <xm:f>Droplist_Terms!$D$2:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000E000000}">
-          <x14:formula1>
-            <xm:f>Droplist_Terms!$I$2:$I$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>R451:R452 Q1:Q520 Q523:Q1048576</xm:sqref>
+          <xm:sqref>E539:E1048576 E2:E538</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Only values from the list can be used" promptTitle="Amino acid type" prompt="Select the mutant amino acid from the list" xr:uid="{00000000-0002-0000-0000-00000F000000}">
           <x14:formula1>
             <xm:f>Droplist_Terms!$B$2:$B$42</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L19999</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Site / Bond / SNP" prompt="A Site / Bond / SNP that has been inserted or removed by mutation._x000a_Optional field, typically only used when the mutant AA is not A or L." xr:uid="{00000000-0002-0000-0000-00000C000000}">
-          <x14:formula1>
-            <xm:f>Droplist_Terms!$G$2:$G$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2:O101 O103:O1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6FB0F3CC-5DA9-3745-AAA9-5F913945D9DC}">
-          <x14:formula1>
-            <xm:f>Droplist_Terms!$I$2:$I$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q521:Q522</xm:sqref>
+          <xm:sqref>L539:L19999 L2:L538</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>